<commit_message>
proposal korean ver upload
</commit_message>
<xml_diff>
--- a/Documents/캡스톤_일정표.xlsx
+++ b/Documents/캡스톤_일정표.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ\Documents\GitHub\capstone-design_2019\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D704A69A-F243-4487-8CBD-1EC4F25A332A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6B2C41-85D7-4333-A89B-7CCC695842C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9564" xr2:uid="{23FAAC4D-BD8D-495D-A2DF-99B8E27B98E0}"/>
   </bookViews>
@@ -32,75 +32,78 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>관련 내용 학습, SRS 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인 기능 구현 및 DB 연동</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>혈당수치 기록 기능 구현 및 DB 연동</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>투약 관련 기록 기능 구현 및 DB 연동</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>식단 기록 기능 구현 및 DB 연동</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>심리상태 분석 기능 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>심리상태 기록 및 저장 기능 구현 및 DB 연동</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>테스트</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중간데모</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>최종데모</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>안드로이드 GUI 구현 및 수정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>3월</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4월</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중간고사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5월</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>6월</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>암호화 기능</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가 기능 구현</t>
+    <t>Related contents acquisition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement Android GUI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement psychological analysis function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement writing psychological state function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement log-in function &amp; DB linking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement blood glucose level function &amp; DB linking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement medication administration function &amp; DB linking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement diet management function &amp; DB linking</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement encryption function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement additional function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Testing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Midterm
+Exam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Midterm
+Demo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Final
+Demo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>March</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>April</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>May</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>June</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -108,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +132,14 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -231,28 +242,34 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -265,11 +282,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,297 +608,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607BE8EA-432F-45C4-B72D-21A015449CEA}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="39.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="8"/>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3">
         <v>11</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="L2" s="3">
         <v>12</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="8" t="s">
+      <c r="M2" s="3">
+        <v>13</v>
+      </c>
+      <c r="N2" s="3">
         <v>14</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4">
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4">
-        <v>12</v>
-      </c>
-      <c r="M2" s="4">
-        <v>13</v>
-      </c>
-      <c r="N2" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" s="13"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="J1:M1"/>
     <mergeCell ref="G3:G13"/>
     <mergeCell ref="N3:N13"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="H3:H13"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>